<commit_message>
Checkpoint: Vocacional + dashboard Projeto21 (Janela de Johari)
</commit_message>
<xml_diff>
--- a/apps/projeto21/Arqs_auxiliares/Projeto21_FAMILIA_codificada.xlsx
+++ b/apps/projeto21/Arqs_auxiliares/Projeto21_FAMILIA_codificada.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wanderley\Apps\escola_no_ar_site\apps\projeto21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wanderley\Apps\escola_no_ar_site\apps\projeto21\Arqs_auxiliares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C226FF2-3089-4FB6-9CDF-4D3B94549612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E8380C-6C66-4414-8E0A-49BB949A1472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7470" yWindow="915" windowWidth="12195" windowHeight="10485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Familia" sheetId="1" r:id="rId1"/>
@@ -39,18 +39,12 @@
     <t>Area</t>
   </si>
   <si>
-    <t>Dimensao</t>
-  </si>
-  <si>
     <t>Estrategia</t>
   </si>
   <si>
     <t>OrdemArea</t>
   </si>
   <si>
-    <t>OrdemDimensao</t>
-  </si>
-  <si>
     <t>OrdemEstrategia</t>
   </si>
   <si>
@@ -297,12 +291,6 @@
     <t>Conversar sobre como você pode colaborar com as finanças familiares com responsabilidade.</t>
   </si>
   <si>
-    <t>quant-intervalo</t>
-  </si>
-  <si>
-    <t>unid-intervfalo</t>
-  </si>
-  <si>
     <t>Ajudar em uma tarefa de casa sem que me peçam. Definir a tarefa.</t>
   </si>
   <si>
@@ -346,6 +334,18 @@
   </si>
   <si>
     <t>Descrição da Frequência</t>
+  </si>
+  <si>
+    <t>Nivel</t>
+  </si>
+  <si>
+    <t>OrdemNivel</t>
+  </si>
+  <si>
+    <t>CadenciaNum</t>
+  </si>
+  <si>
+    <t>CadenciaUnid</t>
   </si>
 </sst>
 </file>
@@ -737,8 +737,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:L8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,62 +754,62 @@
     <col min="15" max="15" width="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
@@ -824,13 +824,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K2" s="6">
         <v>2</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M2" s="4" t="str">
         <f>LEFT(A2,2)&amp;LEFT(B2,1)&amp;TEXT(F2,"000")&amp;"-"&amp;(G2)&amp;H2&amp;(K2)&amp;L2</f>
@@ -847,13 +847,13 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -868,35 +868,35 @@
         <v>1</v>
       </c>
       <c r="H3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="6">
+        <v>3</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="K3" s="6">
-        <v>3</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="N3" s="4">
         <f t="shared" ref="N3:N38" si="0">IF(B3="Básico",1,IF(B3="Desafio",2,IF(B3="Avançado",3)))</f>
         <v>1</v>
       </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:O39" si="1">IF(G3=0,"O dia inteiro",IF(G3=1,"Uma vez",TEXT(G3,"0")&amp;" vezes")&amp;" por "&amp;IF(LOWER(H3)="d","dia","semana"))&amp;IF(AND(ISNUMBER(I3),I3&gt;0),", a cada "&amp;TEXT(I2,"0")&amp;" "&amp;IF(I2=1,IF(LOWER(J3)="d","dia","semana"),IF(LOWER(J3)="d","dias","semanas"))&amp;",","")&amp;" por um período de "&amp;TEXT(K3,"0")&amp;" "&amp;IF(K3=1,IF(LOWER(L3)="d","dia","semana"),IF(LOWER(L3)="d","dias","semanas"))</f>
+        <f t="shared" ref="O3:O38" si="1">IF(G3=0,"O dia inteiro",IF(G3=1,"Uma vez",TEXT(G3,"0")&amp;" vezes")&amp;" por "&amp;IF(LOWER(H3)="d","dia","semana"))&amp;IF(AND(ISNUMBER(I3),I3&gt;0),", a cada "&amp;TEXT(I2,"0")&amp;" "&amp;IF(I2=1,IF(LOWER(J3)="d","dia","semana"),IF(LOWER(J3)="d","dias","semanas"))&amp;",","")&amp;" por um período de "&amp;TEXT(K3,"0")&amp;" "&amp;IF(K3=1,IF(LOWER(L3)="d","dia","semana"),IF(LOWER(L3)="d","dias","semanas"))</f>
         <v>Uma vez por dia por um período de 3 dias</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -911,16 +911,16 @@
         <v>1</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K4" s="6">
         <v>2</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N4" s="4">
         <f t="shared" si="0"/>
@@ -933,13 +933,13 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -954,16 +954,16 @@
         <v>2</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K5" s="6">
         <v>4</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N5" s="4">
         <f t="shared" si="0"/>
@@ -976,13 +976,13 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -997,16 +997,16 @@
         <v>0</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K6" s="6">
         <v>7</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N6" s="4">
         <f t="shared" si="0"/>
@@ -1019,13 +1019,13 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -1040,22 +1040,22 @@
         <v>1</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I7" s="6">
         <v>2</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K7" s="6">
         <v>7</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N7" s="4">
         <f t="shared" si="0"/>
@@ -1068,13 +1068,13 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
@@ -1089,22 +1089,22 @@
         <v>1</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I8" s="6">
         <v>3</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K8" s="6">
         <v>6</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N8" s="4">
         <f t="shared" si="0"/>
@@ -1117,13 +1117,13 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -1138,16 +1138,16 @@
         <v>1</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K9" s="6">
         <v>7</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N9" s="4">
         <f t="shared" si="0"/>
@@ -1160,13 +1160,13 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -1181,22 +1181,22 @@
         <v>1</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I10" s="6">
         <v>2</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K10" s="6">
         <v>6</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N10" s="4">
         <f t="shared" si="0"/>
@@ -1209,13 +1209,13 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -1230,22 +1230,22 @@
         <v>1</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I11" s="6">
         <v>3</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K11" s="6">
         <v>6</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N11" s="4">
         <f t="shared" si="0"/>
@@ -1258,13 +1258,13 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -1279,16 +1279,16 @@
         <v>1</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K12" s="6">
         <v>1</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N12" s="4">
         <f t="shared" si="0"/>
@@ -1301,13 +1301,13 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -1322,16 +1322,16 @@
         <v>1</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K13" s="6">
         <v>2</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N13" s="4">
         <f t="shared" si="0"/>
@@ -1344,13 +1344,13 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
       <c r="C14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -1365,16 +1365,16 @@
         <v>1</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K14" s="6">
         <v>1</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N14" s="4">
         <f t="shared" si="0"/>
@@ -1387,13 +1387,13 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -1408,16 +1408,16 @@
         <v>1</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K15" s="6">
         <v>2</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="N15" s="4">
         <f t="shared" si="0"/>
@@ -1430,13 +1430,13 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
         <v>11</v>
       </c>
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -1451,16 +1451,16 @@
         <v>1</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K16" s="6">
         <v>1</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="N16" s="4">
         <f t="shared" si="0"/>
@@ -1473,13 +1473,13 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
         <v>11</v>
       </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
@@ -1494,16 +1494,16 @@
         <v>1</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K17" s="6">
         <v>7</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N17" s="4">
         <f t="shared" si="0"/>
@@ -1516,13 +1516,13 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -1537,22 +1537,22 @@
         <v>1</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I18" s="6">
         <v>3</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K18" s="6">
         <v>2</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N18" s="4">
         <f t="shared" si="0"/>
@@ -1565,13 +1565,13 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
         <v>11</v>
       </c>
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
@@ -1586,16 +1586,16 @@
         <v>1</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K19" s="6">
         <v>1</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N19" s="4">
         <f t="shared" si="0"/>
@@ -1608,13 +1608,13 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
         <v>11</v>
       </c>
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -1629,16 +1629,16 @@
         <v>1</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K20" s="6">
         <v>7</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N20" s="4">
         <f t="shared" si="0"/>
@@ -1651,13 +1651,13 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
         <v>11</v>
       </c>
-      <c r="B21" t="s">
-        <v>13</v>
-      </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -1672,16 +1672,16 @@
         <v>1</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K21" s="6">
         <v>1</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N21" s="4">
         <f t="shared" si="0"/>
@@ -1694,13 +1694,13 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
         <v>11</v>
       </c>
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
@@ -1715,22 +1715,22 @@
         <v>1</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I22" s="6">
         <v>1</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K22" s="6">
         <v>7</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N22" s="4">
         <f t="shared" si="0"/>
@@ -1743,13 +1743,13 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
         <v>11</v>
       </c>
-      <c r="B23" t="s">
-        <v>13</v>
-      </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D23" s="4">
         <v>1</v>
@@ -1764,16 +1764,16 @@
         <v>1</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K23" s="6">
         <v>7</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N23" s="4">
         <f t="shared" si="0"/>
@@ -1786,13 +1786,13 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
@@ -1807,16 +1807,16 @@
         <v>1</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K24" s="6">
         <v>2</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N24" s="4">
         <f t="shared" si="0"/>
@@ -1829,13 +1829,13 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D25" s="4">
         <v>1</v>
@@ -1850,16 +1850,16 @@
         <v>1</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K25" s="6">
         <v>4</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N25" s="4">
         <f t="shared" si="0"/>
@@ -1872,13 +1872,13 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D26" s="4">
         <v>1</v>
@@ -1893,16 +1893,16 @@
         <v>1</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K26" s="6">
         <v>2</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N26" s="4">
         <f t="shared" si="0"/>
@@ -1915,13 +1915,13 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D27" s="4">
         <v>1</v>
@@ -1936,16 +1936,16 @@
         <v>1</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K27" s="6">
         <v>4</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N27" s="4">
         <f t="shared" si="0"/>
@@ -1958,13 +1958,13 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D28" s="4">
         <v>1</v>
@@ -1979,16 +1979,16 @@
         <v>1</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K28" s="6">
         <v>3</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N28" s="4">
         <f t="shared" si="0"/>
@@ -2001,13 +2001,13 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D29" s="4">
         <v>1</v>
@@ -2022,16 +2022,16 @@
         <v>1</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K29" s="6">
         <v>3</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N29" s="4">
         <f t="shared" si="0"/>
@@ -2044,13 +2044,13 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D30" s="4">
         <v>1</v>
@@ -2065,16 +2065,16 @@
         <v>1</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K30" s="6">
         <v>1</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N30" s="4">
         <f t="shared" si="0"/>
@@ -2087,13 +2087,13 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D31" s="4">
         <v>1</v>
@@ -2108,16 +2108,16 @@
         <v>1</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K31" s="6">
         <v>2</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N31" s="4">
         <f t="shared" si="0"/>
@@ -2130,13 +2130,13 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D32" s="4">
         <v>1</v>
@@ -2151,16 +2151,16 @@
         <v>1</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K32" s="6">
         <v>4</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="N32" s="4">
         <f t="shared" si="0"/>
@@ -2173,13 +2173,13 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D33" s="4">
         <v>1</v>
@@ -2194,16 +2194,16 @@
         <v>1</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K33" s="6">
         <v>4</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N33" s="4">
         <f t="shared" si="0"/>
@@ -2216,13 +2216,13 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D34" s="4">
         <v>1</v>
@@ -2237,16 +2237,16 @@
         <v>3</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K34" s="6">
         <v>3</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N34" s="4">
         <f t="shared" si="0"/>
@@ -2259,13 +2259,13 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D35" s="4">
         <v>1</v>
@@ -2280,16 +2280,16 @@
         <v>1</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K35" s="6">
         <v>2</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N35" s="4">
         <f t="shared" si="0"/>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D36" s="4">
         <v>1</v>
@@ -2323,16 +2323,16 @@
         <v>1</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K36" s="6">
         <v>3</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="N36" s="4">
         <f t="shared" si="0"/>
@@ -2345,13 +2345,13 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D37" s="4">
         <v>1</v>
@@ -2366,16 +2366,16 @@
         <v>1</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K37" s="6">
         <v>1</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N37" s="4">
         <f t="shared" si="0"/>
@@ -2388,13 +2388,13 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D38" s="4">
         <v>1</v>
@@ -2409,16 +2409,16 @@
         <v>1</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K38" s="6">
         <v>4</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="N38" s="4">
         <f t="shared" si="0"/>
@@ -2451,42 +2451,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>